<commit_message>
adding Star Trek Into Darkness 4k
</commit_message>
<xml_diff>
--- a/Disc-Collection-2024-Master.xlsx
+++ b/Disc-Collection-2024-Master.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\scott\Documents\GitHub\blu-ray-HD-UHD-discs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E072B0E0-D1F9-435A-ADFF-C2E2B3C781A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A96E1A3-8B40-4CE8-B5F6-A62518A857E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D5EF86A-635B-4515-8E7E-20C44429F53C}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Blu-Ray-HD-UHD-List-2024" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Blu-Ray-HD-UHD-List-2024'!$A$1:$H$926</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Blu-Ray-HD-UHD-List-2024'!$A$1:$H$927</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5502" uniqueCount="2091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5507" uniqueCount="2092">
   <si>
     <t>Title</t>
   </si>
@@ -6320,6 +6320,9 @@
   </si>
   <si>
     <t>Arrow Video</t>
+  </si>
+  <si>
+    <t>Star Trek Into Darkness</t>
   </si>
 </sst>
 </file>
@@ -6423,8 +6426,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A19FAC-B236-44A3-BEFE-D1B6209BB30B}" name="Blu_Ray_HD_UHD_List_export_movies" displayName="Blu_Ray_HD_UHD_List_export_movies" ref="A1:H926" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H926" xr:uid="{D8A19FAC-B236-44A3-BEFE-D1B6209BB30B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D8A19FAC-B236-44A3-BEFE-D1B6209BB30B}" name="Blu_Ray_HD_UHD_List_export_movies" displayName="Blu_Ray_HD_UHD_List_export_movies" ref="A1:H927" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H927" xr:uid="{D8A19FAC-B236-44A3-BEFE-D1B6209BB30B}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{17695B57-FAC4-45CE-973A-5BC721E39AB6}" uniqueName="1" name="Title" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{D3D45491-1A09-4440-86D7-CD6C0DF0CA6F}" uniqueName="2" name="Release Date" queryTableFieldId="2" dataDxfId="5"/>
@@ -6736,10 +6739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8ED6D6-3EA2-41AC-8913-E481494C0353}">
-  <dimension ref="A1:H926"/>
+  <dimension ref="A1:H927"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView tabSelected="1" topLeftCell="A753" workbookViewId="0">
+      <selection activeCell="A766" sqref="A766"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11357,25 +11360,25 @@
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A178" s="3" t="s">
+      <c r="A178" t="s">
         <v>2087</v>
       </c>
-      <c r="B178" s="4">
+      <c r="B178" s="2">
         <v>1982</v>
       </c>
-      <c r="C178" s="3" t="s">
+      <c r="C178" t="s">
         <v>288</v>
       </c>
       <c r="D178">
         <v>129</v>
       </c>
-      <c r="E178" s="3" t="s">
+      <c r="E178" t="s">
         <v>1566</v>
       </c>
-      <c r="F178" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G178" s="3" t="s">
+      <c r="F178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178" t="s">
         <v>2090</v>
       </c>
       <c r="H178" s="1">
@@ -11383,25 +11386,25 @@
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A179" s="3" t="s">
+      <c r="A179" t="s">
         <v>2088</v>
       </c>
-      <c r="B179" s="4">
+      <c r="B179" s="2">
         <v>1984</v>
       </c>
-      <c r="C179" s="3" t="s">
+      <c r="C179" t="s">
         <v>2089</v>
       </c>
       <c r="D179">
         <v>101</v>
       </c>
-      <c r="E179" s="3" t="s">
+      <c r="E179" t="s">
         <v>1571</v>
       </c>
-      <c r="F179" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G179" s="3" t="s">
+      <c r="F179" t="s">
+        <v>12</v>
+      </c>
+      <c r="G179" t="s">
         <v>2090</v>
       </c>
       <c r="H179" s="1">
@@ -26637,77 +26640,77 @@
       <c r="F765" t="s">
         <v>12</v>
       </c>
-      <c r="G765" t="s">
-        <v>13</v>
+      <c r="G765" s="3" t="s">
+        <v>860</v>
       </c>
       <c r="H765" s="1">
         <v>43115</v>
       </c>
     </row>
     <row r="766" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A766" t="s">
-        <v>1786</v>
-      </c>
-      <c r="B766" s="2" t="s">
-        <v>15</v>
+      <c r="A766" s="3" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B766" s="4">
+        <v>2013</v>
       </c>
       <c r="C766" t="s">
-        <v>734</v>
+        <v>1785</v>
       </c>
       <c r="D766">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="E766" t="s">
-        <v>740</v>
-      </c>
-      <c r="F766" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F766" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="G766" t="s">
-        <v>13</v>
+      <c r="G766" s="3" t="s">
+        <v>860</v>
       </c>
       <c r="H766" s="1">
-        <v>43115</v>
+        <v>45368</v>
       </c>
     </row>
     <row r="767" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A767" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="B767" s="2" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="C767" t="s">
-        <v>246</v>
+        <v>1785</v>
       </c>
       <c r="D767">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E767" t="s">
-        <v>163</v>
+        <v>740</v>
       </c>
       <c r="F767" t="s">
         <v>37</v>
       </c>
-      <c r="G767" t="s">
-        <v>13</v>
+      <c r="G767" s="3" t="s">
+        <v>860</v>
       </c>
       <c r="H767" s="1">
-        <v>44156</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="768" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A768" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="B768" s="2" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="C768" t="s">
         <v>246</v>
       </c>
       <c r="D768">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E768" t="s">
         <v>163</v>
@@ -26724,16 +26727,16 @@
     </row>
     <row r="769" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A769" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B769" s="2" t="s">
-        <v>731</v>
+        <v>68</v>
       </c>
       <c r="C769" t="s">
         <v>246</v>
       </c>
       <c r="D769">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E769" t="s">
         <v>163</v>
@@ -26750,16 +26753,16 @@
     </row>
     <row r="770" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A770" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B770" s="2" t="s">
-        <v>121</v>
+        <v>731</v>
       </c>
       <c r="C770" t="s">
         <v>246</v>
       </c>
       <c r="D770">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="E770" t="s">
         <v>163</v>
@@ -26776,28 +26779,28 @@
     </row>
     <row r="771" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A771" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B771" s="2" t="s">
-        <v>1588</v>
+        <v>121</v>
       </c>
       <c r="C771" t="s">
         <v>246</v>
       </c>
       <c r="D771">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="E771" t="s">
-        <v>1327</v>
+        <v>163</v>
       </c>
       <c r="F771" t="s">
         <v>37</v>
       </c>
       <c r="G771" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
       <c r="H771" s="1">
-        <v>43918</v>
+        <v>44156</v>
       </c>
     </row>
     <row r="772" spans="1:8" x14ac:dyDescent="0.3">
@@ -26820,27 +26823,27 @@
         <v>37</v>
       </c>
       <c r="G772" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="H772" s="1">
-        <v>44156</v>
+        <v>43918</v>
       </c>
     </row>
     <row r="773" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A773" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B773" s="2" t="s">
-        <v>206</v>
+        <v>1588</v>
       </c>
       <c r="C773" t="s">
         <v>246</v>
       </c>
       <c r="D773">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="E773" t="s">
-        <v>1793</v>
+        <v>1327</v>
       </c>
       <c r="F773" t="s">
         <v>37</v>
@@ -26854,19 +26857,19 @@
     </row>
     <row r="774" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A774" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="B774" s="2" t="s">
-        <v>485</v>
+        <v>206</v>
       </c>
       <c r="C774" t="s">
         <v>246</v>
       </c>
       <c r="D774">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E774" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="F774" t="s">
         <v>37</v>
@@ -26880,19 +26883,19 @@
     </row>
     <row r="775" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A775" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
       <c r="B775" s="2" t="s">
-        <v>320</v>
+        <v>485</v>
       </c>
       <c r="C775" t="s">
-        <v>707</v>
+        <v>246</v>
       </c>
       <c r="D775">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E775" t="s">
-        <v>1327</v>
+        <v>1795</v>
       </c>
       <c r="F775" t="s">
         <v>37</v>
@@ -26906,19 +26909,19 @@
     </row>
     <row r="776" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A776" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B776" s="2" t="s">
-        <v>1371</v>
+        <v>320</v>
       </c>
       <c r="C776" t="s">
-        <v>246</v>
+        <v>707</v>
       </c>
       <c r="D776">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="E776" t="s">
-        <v>1798</v>
+        <v>1327</v>
       </c>
       <c r="F776" t="s">
         <v>37</v>
@@ -26932,10 +26935,10 @@
     </row>
     <row r="777" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A777" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="B777" s="2" t="s">
-        <v>136</v>
+        <v>1371</v>
       </c>
       <c r="C777" t="s">
         <v>246</v>
@@ -26950,157 +26953,157 @@
         <v>37</v>
       </c>
       <c r="G777" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
       <c r="H777" s="1">
-        <v>43195</v>
+        <v>44156</v>
       </c>
     </row>
     <row r="778" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A778" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B778" s="2" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
       <c r="C778" t="s">
-        <v>311</v>
+        <v>246</v>
       </c>
       <c r="D778">
-        <v>4316</v>
+        <v>152</v>
       </c>
       <c r="E778" t="s">
-        <v>1801</v>
+        <v>1798</v>
       </c>
       <c r="F778" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G778" t="s">
-        <v>426</v>
+        <v>204</v>
       </c>
       <c r="H778" s="1">
-        <v>43143</v>
+        <v>43195</v>
       </c>
     </row>
     <row r="779" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A779" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="B779" s="2" t="s">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="C779" t="s">
-        <v>1803</v>
+        <v>311</v>
       </c>
       <c r="D779">
-        <v>129</v>
+        <v>4316</v>
       </c>
       <c r="E779" t="s">
-        <v>1804</v>
+        <v>1801</v>
       </c>
       <c r="F779" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G779" t="s">
-        <v>13</v>
+        <v>426</v>
       </c>
       <c r="H779" s="1">
-        <v>43133</v>
+        <v>43143</v>
       </c>
     </row>
     <row r="780" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A780" t="s">
-        <v>1805</v>
+        <v>1802</v>
       </c>
       <c r="B780" s="2" t="s">
-        <v>206</v>
+        <v>81</v>
       </c>
       <c r="C780" t="s">
-        <v>146</v>
+        <v>1803</v>
       </c>
       <c r="D780">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="E780" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="F780" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G780" t="s">
-        <v>216</v>
+        <v>13</v>
       </c>
       <c r="H780" s="1">
-        <v>43250</v>
+        <v>43133</v>
       </c>
     </row>
     <row r="781" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A781" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="B781" s="2" t="s">
-        <v>72</v>
+        <v>206</v>
       </c>
       <c r="C781" t="s">
-        <v>1808</v>
+        <v>146</v>
       </c>
       <c r="D781">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E781" t="s">
-        <v>1533</v>
+        <v>1806</v>
       </c>
       <c r="F781" t="s">
         <v>12</v>
       </c>
       <c r="G781" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
       <c r="H781" s="1">
-        <v>43115</v>
+        <v>43250</v>
       </c>
     </row>
     <row r="782" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A782" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
       <c r="B782" s="2" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C782" t="s">
-        <v>229</v>
+        <v>1808</v>
       </c>
       <c r="D782">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E782" t="s">
-        <v>597</v>
+        <v>1533</v>
       </c>
       <c r="F782" t="s">
         <v>12</v>
       </c>
       <c r="G782" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="H782" s="1">
-        <v>44351</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="783" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A783" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B783" s="2" t="s">
-        <v>731</v>
+        <v>38</v>
       </c>
       <c r="C783" t="s">
-        <v>586</v>
+        <v>229</v>
       </c>
       <c r="D783">
-        <v>235</v>
+        <v>89</v>
       </c>
       <c r="E783" t="s">
-        <v>1811</v>
+        <v>597</v>
       </c>
       <c r="F783" t="s">
         <v>12</v>
@@ -27109,160 +27112,160 @@
         <v>13</v>
       </c>
       <c r="H783" s="1">
-        <v>44258</v>
+        <v>44351</v>
       </c>
     </row>
     <row r="784" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A784" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="B784" s="2" t="s">
-        <v>182</v>
+        <v>731</v>
       </c>
       <c r="C784" t="s">
-        <v>1813</v>
+        <v>586</v>
       </c>
       <c r="D784">
-        <v>107</v>
+        <v>235</v>
       </c>
       <c r="E784" t="s">
-        <v>862</v>
+        <v>1811</v>
       </c>
       <c r="F784" t="s">
         <v>12</v>
       </c>
       <c r="G784" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="H784" s="1">
-        <v>43115</v>
+        <v>44258</v>
       </c>
     </row>
     <row r="785" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A785" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
       <c r="B785" s="2" t="s">
-        <v>485</v>
+        <v>182</v>
       </c>
       <c r="C785" t="s">
-        <v>718</v>
+        <v>1813</v>
       </c>
       <c r="D785">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E785" t="s">
-        <v>83</v>
+        <v>862</v>
       </c>
       <c r="F785" t="s">
         <v>12</v>
       </c>
       <c r="G785" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="H785" s="1">
-        <v>43271</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="786" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A786" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B786" s="2" t="s">
-        <v>68</v>
+        <v>485</v>
       </c>
       <c r="C786" t="s">
-        <v>114</v>
+        <v>718</v>
       </c>
       <c r="D786">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E786" t="s">
-        <v>1816</v>
+        <v>83</v>
       </c>
       <c r="F786" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G786" t="s">
         <v>13</v>
       </c>
       <c r="H786" s="1">
-        <v>43338</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="787" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A787" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="B787" s="2" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="C787" t="s">
-        <v>568</v>
+        <v>114</v>
       </c>
       <c r="D787">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="E787" t="s">
-        <v>50</v>
+        <v>1816</v>
       </c>
       <c r="F787" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G787" t="s">
         <v>13</v>
       </c>
       <c r="H787" s="1">
-        <v>43424</v>
+        <v>43338</v>
       </c>
     </row>
     <row r="788" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A788" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="B788" s="2" t="s">
-        <v>1819</v>
+        <v>99</v>
       </c>
       <c r="C788" t="s">
-        <v>1653</v>
+        <v>568</v>
       </c>
       <c r="D788">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="E788" t="s">
-        <v>1654</v>
+        <v>50</v>
       </c>
       <c r="F788" t="s">
         <v>12</v>
       </c>
       <c r="G788" t="s">
-        <v>327</v>
+        <v>13</v>
       </c>
       <c r="H788" s="1">
-        <v>43115</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="789" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A789" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="B789" s="2" t="s">
-        <v>68</v>
+        <v>1819</v>
       </c>
       <c r="C789" t="s">
-        <v>105</v>
+        <v>1653</v>
       </c>
       <c r="D789">
-        <v>103</v>
+        <v>130</v>
       </c>
       <c r="E789" t="s">
-        <v>303</v>
+        <v>1654</v>
       </c>
       <c r="F789" t="s">
         <v>12</v>
       </c>
       <c r="G789" t="s">
-        <v>79</v>
+        <v>327</v>
       </c>
       <c r="H789" s="1">
         <v>43115</v>
@@ -27270,16 +27273,16 @@
     </row>
     <row r="790" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A790" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="B790" s="2" t="s">
-        <v>317</v>
+        <v>68</v>
       </c>
       <c r="C790" t="s">
-        <v>1822</v>
+        <v>105</v>
       </c>
       <c r="D790">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="E790" t="s">
         <v>303</v>
@@ -27291,56 +27294,56 @@
         <v>79</v>
       </c>
       <c r="H790" s="1">
-        <v>43303</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="791" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A791" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="B791" s="2" t="s">
-        <v>275</v>
+        <v>317</v>
       </c>
       <c r="C791" t="s">
-        <v>156</v>
+        <v>1822</v>
       </c>
       <c r="D791">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E791" t="s">
-        <v>1824</v>
+        <v>303</v>
       </c>
       <c r="F791" t="s">
         <v>12</v>
       </c>
       <c r="G791" t="s">
-        <v>153</v>
+        <v>79</v>
       </c>
       <c r="H791" s="1">
-        <v>43115</v>
+        <v>43303</v>
       </c>
     </row>
     <row r="792" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A792" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="B792" s="2" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="C792" t="s">
-        <v>1826</v>
+        <v>156</v>
       </c>
       <c r="D792">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E792" t="s">
-        <v>1827</v>
+        <v>1824</v>
       </c>
       <c r="F792" t="s">
         <v>12</v>
       </c>
       <c r="G792" t="s">
-        <v>331</v>
+        <v>153</v>
       </c>
       <c r="H792" s="1">
         <v>43115</v>
@@ -27348,25 +27351,25 @@
     </row>
     <row r="793" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A793" t="s">
-        <v>1828</v>
+        <v>1825</v>
       </c>
       <c r="B793" s="2" t="s">
-        <v>694</v>
+        <v>155</v>
       </c>
       <c r="C793" t="s">
-        <v>156</v>
+        <v>1826</v>
       </c>
       <c r="D793">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="E793" t="s">
-        <v>111</v>
+        <v>1827</v>
       </c>
       <c r="F793" t="s">
         <v>12</v>
       </c>
       <c r="G793" t="s">
-        <v>194</v>
+        <v>331</v>
       </c>
       <c r="H793" s="1">
         <v>43115</v>
@@ -27374,120 +27377,120 @@
     </row>
     <row r="794" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A794" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B794" s="2" t="s">
-        <v>1830</v>
+        <v>694</v>
       </c>
       <c r="C794" t="s">
-        <v>1831</v>
+        <v>156</v>
       </c>
       <c r="D794">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E794" t="s">
-        <v>1832</v>
+        <v>111</v>
       </c>
       <c r="F794" t="s">
         <v>12</v>
       </c>
       <c r="G794" t="s">
-        <v>23</v>
+        <v>194</v>
       </c>
       <c r="H794" s="1">
-        <v>43119</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="795" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A795" t="s">
-        <v>1833</v>
+        <v>1829</v>
       </c>
       <c r="B795" s="2" t="s">
-        <v>38</v>
+        <v>1830</v>
       </c>
       <c r="C795" t="s">
-        <v>53</v>
+        <v>1831</v>
       </c>
       <c r="D795">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E795" t="s">
-        <v>143</v>
+        <v>1832</v>
       </c>
       <c r="F795" t="s">
         <v>12</v>
       </c>
       <c r="G795" t="s">
-        <v>168</v>
+        <v>23</v>
       </c>
       <c r="H795" s="1">
-        <v>43115</v>
+        <v>43119</v>
       </c>
     </row>
     <row r="796" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A796" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="B796" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C796" t="s">
-        <v>707</v>
+        <v>53</v>
       </c>
       <c r="D796">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="E796" t="s">
-        <v>600</v>
+        <v>143</v>
       </c>
       <c r="F796" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G796" t="s">
-        <v>18</v>
+        <v>168</v>
       </c>
       <c r="H796" s="1">
-        <v>43858</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="797" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A797" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B797" s="2" t="s">
-        <v>305</v>
+        <v>34</v>
       </c>
       <c r="C797" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
       <c r="D797">
-        <v>99</v>
+        <v>128</v>
       </c>
       <c r="E797" t="s">
-        <v>13</v>
+        <v>600</v>
       </c>
       <c r="F797" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G797" t="s">
-        <v>1651</v>
+        <v>18</v>
       </c>
       <c r="H797" s="1">
-        <v>44024</v>
+        <v>43858</v>
       </c>
     </row>
     <row r="798" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A798" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="B798" s="2" t="s">
-        <v>1837</v>
+        <v>305</v>
       </c>
       <c r="C798" t="s">
         <v>698</v>
       </c>
       <c r="D798">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E798" t="s">
         <v>13</v>
@@ -27504,28 +27507,28 @@
     </row>
     <row r="799" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A799" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
       <c r="B799" s="2" t="s">
-        <v>284</v>
+        <v>1837</v>
       </c>
       <c r="C799" t="s">
-        <v>770</v>
+        <v>698</v>
       </c>
       <c r="D799">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="E799" t="s">
-        <v>126</v>
+        <v>13</v>
       </c>
       <c r="F799" t="s">
         <v>12</v>
       </c>
       <c r="G799" t="s">
-        <v>440</v>
+        <v>1651</v>
       </c>
       <c r="H799" s="1">
-        <v>43228</v>
+        <v>44024</v>
       </c>
     </row>
     <row r="800" spans="1:8" x14ac:dyDescent="0.3">
@@ -27545,143 +27548,143 @@
         <v>126</v>
       </c>
       <c r="F800" t="s">
-        <v>2066</v>
+        <v>12</v>
       </c>
       <c r="G800" t="s">
-        <v>1651</v>
+        <v>440</v>
       </c>
       <c r="H800" s="1">
-        <v>45092</v>
+        <v>43228</v>
       </c>
     </row>
     <row r="801" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A801" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B801" s="2" t="s">
-        <v>52</v>
+        <v>284</v>
       </c>
       <c r="C801" t="s">
-        <v>335</v>
+        <v>770</v>
       </c>
       <c r="D801">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="E801" t="s">
-        <v>392</v>
+        <v>126</v>
       </c>
       <c r="F801" t="s">
-        <v>12</v>
+        <v>2066</v>
       </c>
       <c r="G801" t="s">
-        <v>198</v>
+        <v>1651</v>
       </c>
       <c r="H801" s="1">
-        <v>43115</v>
+        <v>45092</v>
       </c>
     </row>
     <row r="802" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A802" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="B802" s="2" t="s">
-        <v>1841</v>
+        <v>52</v>
       </c>
       <c r="C802" t="s">
-        <v>218</v>
+        <v>335</v>
       </c>
       <c r="D802">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="E802" t="s">
-        <v>13</v>
+        <v>392</v>
       </c>
       <c r="F802" t="s">
         <v>12</v>
       </c>
       <c r="G802" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="H802" s="1">
-        <v>44026</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="803" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A803" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
       <c r="B803" s="2" t="s">
-        <v>124</v>
+        <v>1841</v>
       </c>
       <c r="C803" t="s">
-        <v>335</v>
+        <v>218</v>
       </c>
       <c r="D803">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="E803" t="s">
-        <v>1843</v>
+        <v>13</v>
       </c>
       <c r="F803" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="G803" t="s">
-        <v>1844</v>
+        <v>13</v>
       </c>
       <c r="H803" s="1">
-        <v>43431</v>
+        <v>44026</v>
       </c>
     </row>
     <row r="804" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A804" t="s">
-        <v>1845</v>
+        <v>1842</v>
       </c>
       <c r="B804" s="2" t="s">
-        <v>43</v>
+        <v>124</v>
       </c>
       <c r="C804" t="s">
-        <v>1846</v>
+        <v>335</v>
       </c>
       <c r="D804">
+        <v>0</v>
+      </c>
+      <c r="E804" t="s">
+        <v>1843</v>
+      </c>
+      <c r="F804" t="s">
         <v>102</v>
       </c>
-      <c r="E804" t="s">
-        <v>1061</v>
-      </c>
-      <c r="F804" t="s">
-        <v>12</v>
-      </c>
       <c r="G804" t="s">
-        <v>13</v>
+        <v>1844</v>
       </c>
       <c r="H804" s="1">
-        <v>43695</v>
+        <v>43431</v>
       </c>
     </row>
     <row r="805" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A805" t="s">
-        <v>2073</v>
-      </c>
-      <c r="B805" s="2">
-        <v>2022</v>
+        <v>1845</v>
+      </c>
+      <c r="B805" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="C805" t="s">
-        <v>2078</v>
+        <v>1846</v>
       </c>
       <c r="D805">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E805" t="s">
-        <v>2079</v>
+        <v>1061</v>
       </c>
       <c r="F805" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G805" t="s">
-        <v>2075</v>
+        <v>13</v>
       </c>
       <c r="H805" s="1">
-        <v>45306</v>
+        <v>43695</v>
       </c>
     </row>
     <row r="806" spans="1:8" x14ac:dyDescent="0.3">
@@ -27701,7 +27704,7 @@
         <v>2079</v>
       </c>
       <c r="F806" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G806" t="s">
         <v>2075</v>
@@ -27712,45 +27715,45 @@
     </row>
     <row r="807" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A807" t="s">
-        <v>1847</v>
-      </c>
-      <c r="B807" s="2" t="s">
-        <v>1848</v>
+        <v>2073</v>
+      </c>
+      <c r="B807" s="2">
+        <v>2022</v>
       </c>
       <c r="C807" t="s">
-        <v>110</v>
+        <v>2078</v>
       </c>
       <c r="D807">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="E807" t="s">
-        <v>50</v>
+        <v>2079</v>
       </c>
       <c r="F807" t="s">
         <v>12</v>
       </c>
       <c r="G807" t="s">
-        <v>13</v>
+        <v>2075</v>
       </c>
       <c r="H807" s="1">
-        <v>43424</v>
+        <v>45306</v>
       </c>
     </row>
     <row r="808" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A808" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="B808" s="2" t="s">
-        <v>826</v>
+        <v>1848</v>
       </c>
       <c r="C808" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="D808">
-        <v>5</v>
+        <v>98</v>
       </c>
       <c r="E808" t="s">
-        <v>1171</v>
+        <v>50</v>
       </c>
       <c r="F808" t="s">
         <v>12</v>
@@ -27759,47 +27762,47 @@
         <v>13</v>
       </c>
       <c r="H808" s="1">
-        <v>43271</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="809" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A809" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B809" s="2" t="s">
-        <v>275</v>
+        <v>826</v>
       </c>
       <c r="C809" t="s">
-        <v>554</v>
+        <v>92</v>
       </c>
       <c r="D809">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="E809" t="s">
-        <v>1851</v>
+        <v>1171</v>
       </c>
       <c r="F809" t="s">
         <v>12</v>
       </c>
       <c r="G809" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
       <c r="H809" s="1">
-        <v>43115</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="810" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A810" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
       <c r="B810" s="2" t="s">
-        <v>155</v>
+        <v>275</v>
       </c>
       <c r="C810" t="s">
-        <v>1853</v>
+        <v>554</v>
       </c>
       <c r="D810">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E810" t="s">
         <v>1851</v>
@@ -27808,7 +27811,7 @@
         <v>12</v>
       </c>
       <c r="G810" t="s">
-        <v>327</v>
+        <v>204</v>
       </c>
       <c r="H810" s="1">
         <v>43115</v>
@@ -27816,25 +27819,25 @@
     </row>
     <row r="811" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A811" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="B811" s="2" t="s">
-        <v>1855</v>
+        <v>155</v>
       </c>
       <c r="C811" t="s">
-        <v>1856</v>
+        <v>1853</v>
       </c>
       <c r="D811">
         <v>76</v>
       </c>
       <c r="E811" t="s">
-        <v>1857</v>
+        <v>1851</v>
       </c>
       <c r="F811" t="s">
         <v>12</v>
       </c>
       <c r="G811" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="H811" s="1">
         <v>43115</v>
@@ -27842,25 +27845,25 @@
     </row>
     <row r="812" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A812" t="s">
-        <v>1858</v>
+        <v>1854</v>
       </c>
       <c r="B812" s="2" t="s">
-        <v>9</v>
+        <v>1855</v>
       </c>
       <c r="C812" t="s">
-        <v>1859</v>
+        <v>1856</v>
       </c>
       <c r="D812">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E812" t="s">
-        <v>1473</v>
+        <v>1857</v>
       </c>
       <c r="F812" t="s">
         <v>12</v>
       </c>
       <c r="G812" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="H812" s="1">
         <v>43115</v>
@@ -27868,19 +27871,19 @@
     </row>
     <row r="813" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A813" t="s">
-        <v>1860</v>
+        <v>1858</v>
       </c>
       <c r="B813" s="2" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="C813" t="s">
-        <v>489</v>
+        <v>1859</v>
       </c>
       <c r="D813">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E813" t="s">
-        <v>1861</v>
+        <v>1473</v>
       </c>
       <c r="F813" t="s">
         <v>12</v>
@@ -27894,149 +27897,149 @@
     </row>
     <row r="814" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A814" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="B814" s="2" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
       <c r="C814" t="s">
-        <v>1863</v>
+        <v>489</v>
       </c>
       <c r="D814">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="E814" t="s">
-        <v>1864</v>
+        <v>1861</v>
       </c>
       <c r="F814" t="s">
         <v>12</v>
       </c>
       <c r="G814" t="s">
-        <v>164</v>
+        <v>327</v>
       </c>
       <c r="H814" s="1">
-        <v>43229</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="815" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A815" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="B815" s="2" t="s">
-        <v>485</v>
+        <v>29</v>
       </c>
       <c r="C815" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
       <c r="D815">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="E815" t="s">
-        <v>1867</v>
+        <v>1864</v>
       </c>
       <c r="F815" t="s">
         <v>12</v>
       </c>
       <c r="G815" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="H815" s="1">
-        <v>43271</v>
+        <v>43229</v>
       </c>
     </row>
     <row r="816" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A816" t="s">
-        <v>1868</v>
+        <v>1865</v>
       </c>
       <c r="B816" s="2" t="s">
-        <v>385</v>
+        <v>485</v>
       </c>
       <c r="C816" t="s">
-        <v>1869</v>
+        <v>1866</v>
       </c>
       <c r="D816">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="E816" t="s">
-        <v>1870</v>
+        <v>1867</v>
       </c>
       <c r="F816" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G816" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H816" s="1">
-        <v>43268</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="817" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A817" t="s">
-        <v>1871</v>
+        <v>1868</v>
       </c>
       <c r="B817" s="2" t="s">
-        <v>142</v>
+        <v>385</v>
       </c>
       <c r="C817" t="s">
-        <v>1602</v>
+        <v>1869</v>
       </c>
       <c r="D817">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E817" t="s">
-        <v>1248</v>
+        <v>1870</v>
       </c>
       <c r="F817" t="s">
         <v>37</v>
       </c>
       <c r="G817" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="H817" s="1">
-        <v>44467</v>
+        <v>43268</v>
       </c>
     </row>
     <row r="818" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A818" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B818" s="2" t="s">
-        <v>1873</v>
+        <v>142</v>
       </c>
       <c r="C818" t="s">
+        <v>1602</v>
+      </c>
+      <c r="D818">
         <v>110</v>
       </c>
-      <c r="D818">
-        <v>83</v>
-      </c>
       <c r="E818" t="s">
-        <v>50</v>
+        <v>1248</v>
       </c>
       <c r="F818" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G818" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H818" s="1">
-        <v>43424</v>
+        <v>44467</v>
       </c>
     </row>
     <row r="819" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A819" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="B819" s="2" t="s">
-        <v>435</v>
+        <v>1873</v>
       </c>
       <c r="C819" t="s">
-        <v>762</v>
+        <v>110</v>
       </c>
       <c r="D819">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="E819" t="s">
-        <v>1804</v>
+        <v>50</v>
       </c>
       <c r="F819" t="s">
         <v>12</v>
@@ -28045,24 +28048,24 @@
         <v>13</v>
       </c>
       <c r="H819" s="1">
-        <v>43115</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="820" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A820" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B820" s="2" t="s">
-        <v>305</v>
+        <v>435</v>
       </c>
       <c r="C820" t="s">
-        <v>1876</v>
+        <v>762</v>
       </c>
       <c r="D820">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E820" t="s">
-        <v>50</v>
+        <v>1804</v>
       </c>
       <c r="F820" t="s">
         <v>12</v>
@@ -28071,76 +28074,76 @@
         <v>13</v>
       </c>
       <c r="H820" s="1">
-        <v>43424</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="821" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A821" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="B821" s="2" t="s">
-        <v>155</v>
+        <v>305</v>
       </c>
       <c r="C821" t="s">
-        <v>838</v>
+        <v>1876</v>
       </c>
       <c r="D821">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="E821" t="s">
-        <v>1878</v>
+        <v>50</v>
       </c>
       <c r="F821" t="s">
         <v>12</v>
       </c>
       <c r="G821" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
       <c r="H821" s="1">
-        <v>43115</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="822" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A822" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="B822" s="2" t="s">
-        <v>15</v>
+        <v>155</v>
       </c>
       <c r="C822" t="s">
-        <v>60</v>
+        <v>838</v>
       </c>
       <c r="D822">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="E822" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
       <c r="F822" t="s">
         <v>12</v>
       </c>
       <c r="G822" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="H822" s="1">
-        <v>43268</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="823" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A823" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="B823" s="2" t="s">
-        <v>161</v>
+        <v>15</v>
       </c>
       <c r="C823" t="s">
         <v>60</v>
       </c>
       <c r="D823">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E823" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
       <c r="F823" t="s">
         <v>12</v>
@@ -28149,33 +28152,33 @@
         <v>13</v>
       </c>
       <c r="H823" s="1">
-        <v>43834</v>
+        <v>43268</v>
       </c>
     </row>
     <row r="824" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A824" t="s">
-        <v>2082</v>
-      </c>
-      <c r="B824" s="2">
-        <v>1996</v>
+        <v>1881</v>
+      </c>
+      <c r="B824" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="C824" t="s">
-        <v>2083</v>
+        <v>60</v>
       </c>
       <c r="D824">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E824" t="s">
-        <v>2084</v>
+        <v>1882</v>
       </c>
       <c r="F824" t="s">
         <v>12</v>
       </c>
       <c r="G824" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="H824" s="1">
-        <v>45321</v>
+        <v>43834</v>
       </c>
     </row>
     <row r="825" spans="1:8" x14ac:dyDescent="0.3">
@@ -28195,7 +28198,7 @@
         <v>2084</v>
       </c>
       <c r="F825" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G825" t="s">
         <v>41</v>
@@ -28206,68 +28209,68 @@
     </row>
     <row r="826" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A826" t="s">
-        <v>1883</v>
-      </c>
-      <c r="B826" s="2" t="s">
-        <v>275</v>
+        <v>2082</v>
+      </c>
+      <c r="B826" s="2">
+        <v>1996</v>
       </c>
       <c r="C826" t="s">
-        <v>549</v>
+        <v>2083</v>
       </c>
       <c r="D826">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="E826" t="s">
-        <v>1884</v>
+        <v>2084</v>
       </c>
       <c r="F826" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G826" t="s">
-        <v>1885</v>
+        <v>41</v>
       </c>
       <c r="H826" s="1">
-        <v>43268</v>
+        <v>45321</v>
       </c>
     </row>
     <row r="827" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A827" t="s">
-        <v>1886</v>
+        <v>1883</v>
       </c>
       <c r="B827" s="2" t="s">
-        <v>52</v>
+        <v>275</v>
       </c>
       <c r="C827" t="s">
-        <v>1887</v>
+        <v>549</v>
       </c>
       <c r="D827">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="E827" t="s">
-        <v>257</v>
+        <v>1884</v>
       </c>
       <c r="F827" t="s">
         <v>12</v>
       </c>
       <c r="G827" t="s">
-        <v>756</v>
+        <v>1885</v>
       </c>
       <c r="H827" s="1">
-        <v>43224</v>
+        <v>43268</v>
       </c>
     </row>
     <row r="828" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A828" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
       <c r="B828" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C828" t="s">
-        <v>707</v>
+        <v>1887</v>
       </c>
       <c r="D828">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E828" t="s">
         <v>257</v>
@@ -28279,21 +28282,21 @@
         <v>756</v>
       </c>
       <c r="H828" s="1">
-        <v>43115</v>
+        <v>43224</v>
       </c>
     </row>
     <row r="829" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A829" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B829" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C829" t="s">
         <v>707</v>
       </c>
       <c r="D829">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E829" t="s">
         <v>257</v>
@@ -28310,45 +28313,45 @@
     </row>
     <row r="830" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A830" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B830" s="2" t="s">
-        <v>690</v>
+        <v>9</v>
       </c>
       <c r="C830" t="s">
-        <v>1891</v>
+        <v>707</v>
       </c>
       <c r="D830">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="E830" t="s">
-        <v>50</v>
+        <v>257</v>
       </c>
       <c r="F830" t="s">
         <v>12</v>
       </c>
       <c r="G830" t="s">
-        <v>13</v>
+        <v>756</v>
       </c>
       <c r="H830" s="1">
-        <v>43424</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="831" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A831" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
       <c r="B831" s="2" t="s">
-        <v>192</v>
+        <v>690</v>
       </c>
       <c r="C831" t="s">
-        <v>246</v>
+        <v>1891</v>
       </c>
       <c r="D831">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="E831" t="s">
-        <v>1893</v>
+        <v>50</v>
       </c>
       <c r="F831" t="s">
         <v>12</v>
@@ -28357,24 +28360,24 @@
         <v>13</v>
       </c>
       <c r="H831" s="1">
-        <v>43271</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="832" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A832" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="B832" s="2" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="C832" t="s">
         <v>246</v>
       </c>
       <c r="D832">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="E832" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="F832" t="s">
         <v>12</v>
@@ -28388,19 +28391,19 @@
     </row>
     <row r="833" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A833" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
       <c r="B833" s="2" t="s">
-        <v>275</v>
+        <v>155</v>
       </c>
       <c r="C833" t="s">
-        <v>438</v>
+        <v>246</v>
       </c>
       <c r="D833">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="E833" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="F833" t="s">
         <v>12</v>
@@ -28409,24 +28412,24 @@
         <v>13</v>
       </c>
       <c r="H833" s="1">
-        <v>43115</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="834" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A834" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
       <c r="B834" s="2" t="s">
-        <v>1899</v>
+        <v>275</v>
       </c>
       <c r="C834" t="s">
-        <v>1900</v>
+        <v>438</v>
       </c>
       <c r="D834">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E834" t="s">
-        <v>1901</v>
+        <v>1897</v>
       </c>
       <c r="F834" t="s">
         <v>12</v>
@@ -28435,24 +28438,24 @@
         <v>13</v>
       </c>
       <c r="H834" s="1">
-        <v>43271</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="835" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A835" t="s">
-        <v>1902</v>
+        <v>1898</v>
       </c>
       <c r="B835" s="2" t="s">
-        <v>155</v>
+        <v>1899</v>
       </c>
       <c r="C835" t="s">
-        <v>453</v>
+        <v>1900</v>
       </c>
       <c r="D835">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E835" t="s">
-        <v>446</v>
+        <v>1901</v>
       </c>
       <c r="F835" t="s">
         <v>12</v>
@@ -28461,24 +28464,24 @@
         <v>13</v>
       </c>
       <c r="H835" s="1">
-        <v>43115</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="836" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A836" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B836" s="2" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="C836" t="s">
-        <v>314</v>
+        <v>453</v>
       </c>
       <c r="D836">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="E836" t="s">
-        <v>1904</v>
+        <v>446</v>
       </c>
       <c r="F836" t="s">
         <v>12</v>
@@ -28487,76 +28490,76 @@
         <v>13</v>
       </c>
       <c r="H836" s="1">
-        <v>44496</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="837" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A837" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="B837" s="2" t="s">
-        <v>63</v>
+        <v>142</v>
       </c>
       <c r="C837" t="s">
-        <v>389</v>
+        <v>314</v>
       </c>
       <c r="D837">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E837" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="F837" t="s">
         <v>12</v>
       </c>
       <c r="G837" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="H837" s="1">
-        <v>43115</v>
+        <v>44496</v>
       </c>
     </row>
     <row r="838" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A838" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="B838" s="2" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="C838" t="s">
-        <v>928</v>
+        <v>389</v>
       </c>
       <c r="D838">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E838" t="s">
-        <v>373</v>
+        <v>1906</v>
       </c>
       <c r="F838" t="s">
         <v>12</v>
       </c>
       <c r="G838" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="H838" s="1">
-        <v>43271</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="839" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A839" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B839" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C839" t="s">
-        <v>1909</v>
+        <v>928</v>
       </c>
       <c r="D839">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="E839" t="s">
-        <v>307</v>
+        <v>373</v>
       </c>
       <c r="F839" t="s">
         <v>12</v>
@@ -28565,30 +28568,30 @@
         <v>13</v>
       </c>
       <c r="H839" s="1">
-        <v>43115</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="840" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A840" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="B840" s="2" t="s">
-        <v>1911</v>
+        <v>113</v>
       </c>
       <c r="C840" t="s">
-        <v>573</v>
+        <v>1909</v>
       </c>
       <c r="D840">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="E840" t="s">
-        <v>1912</v>
+        <v>307</v>
       </c>
       <c r="F840" t="s">
         <v>12</v>
       </c>
       <c r="G840" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="H840" s="1">
         <v>43115</v>
@@ -28596,45 +28599,45 @@
     </row>
     <row r="841" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A841" t="s">
-        <v>1913</v>
+        <v>1910</v>
       </c>
       <c r="B841" s="2" t="s">
-        <v>448</v>
+        <v>1911</v>
       </c>
       <c r="C841" t="s">
-        <v>60</v>
+        <v>573</v>
       </c>
       <c r="D841">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="E841" t="s">
-        <v>454</v>
+        <v>1912</v>
       </c>
       <c r="F841" t="s">
         <v>12</v>
       </c>
       <c r="G841" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="H841" s="1">
-        <v>43847</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="842" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A842" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B842" s="2" t="s">
-        <v>128</v>
+        <v>448</v>
       </c>
       <c r="C842" t="s">
-        <v>925</v>
+        <v>60</v>
       </c>
       <c r="D842">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E842" t="s">
-        <v>83</v>
+        <v>454</v>
       </c>
       <c r="F842" t="s">
         <v>12</v>
@@ -28643,7 +28646,7 @@
         <v>13</v>
       </c>
       <c r="H842" s="1">
-        <v>43271</v>
+        <v>43847</v>
       </c>
     </row>
     <row r="843" spans="1:8" x14ac:dyDescent="0.3">
@@ -28657,114 +28660,114 @@
         <v>925</v>
       </c>
       <c r="D843">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E843" t="s">
         <v>83</v>
       </c>
       <c r="F843" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G843" t="s">
-        <v>1710</v>
+        <v>13</v>
       </c>
       <c r="H843" s="1">
-        <v>43116</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="844" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A844" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B844" s="2" t="s">
-        <v>1916</v>
+        <v>128</v>
       </c>
       <c r="C844" t="s">
-        <v>1917</v>
+        <v>925</v>
       </c>
       <c r="D844">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="E844" t="s">
-        <v>544</v>
+        <v>83</v>
       </c>
       <c r="F844" t="s">
         <v>37</v>
       </c>
       <c r="G844" t="s">
-        <v>23</v>
+        <v>1710</v>
       </c>
       <c r="H844" s="1">
-        <v>43358</v>
+        <v>43116</v>
       </c>
     </row>
     <row r="845" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A845" t="s">
-        <v>1918</v>
+        <v>1915</v>
       </c>
       <c r="B845" s="2" t="s">
-        <v>9</v>
+        <v>1916</v>
       </c>
       <c r="C845" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
       <c r="D845">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E845" t="s">
-        <v>1920</v>
+        <v>544</v>
       </c>
       <c r="F845" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G845" t="s">
-        <v>824</v>
+        <v>23</v>
       </c>
       <c r="H845" s="1">
-        <v>43115</v>
+        <v>43358</v>
       </c>
     </row>
     <row r="846" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A846" t="s">
-        <v>1921</v>
+        <v>1918</v>
       </c>
       <c r="B846" s="2" t="s">
-        <v>305</v>
+        <v>9</v>
       </c>
       <c r="C846" t="s">
-        <v>335</v>
+        <v>1919</v>
       </c>
       <c r="D846">
-        <v>650</v>
+        <v>92</v>
       </c>
       <c r="E846" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="F846" t="s">
-        <v>102</v>
+        <v>12</v>
       </c>
       <c r="G846" t="s">
-        <v>1844</v>
+        <v>824</v>
       </c>
       <c r="H846" s="1">
-        <v>43431</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="847" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A847" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
       <c r="B847" s="2" t="s">
-        <v>161</v>
+        <v>305</v>
       </c>
       <c r="C847" t="s">
         <v>335</v>
       </c>
       <c r="D847">
-        <v>780</v>
+        <v>650</v>
       </c>
       <c r="E847" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="F847" t="s">
         <v>102</v>
@@ -28778,19 +28781,19 @@
     </row>
     <row r="848" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A848" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
       <c r="B848" s="2" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="C848" t="s">
-        <v>421</v>
+        <v>335</v>
       </c>
       <c r="D848">
         <v>780</v>
       </c>
       <c r="E848" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="F848" t="s">
         <v>102</v>
@@ -28804,19 +28807,19 @@
     </row>
     <row r="849" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A849" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
       <c r="B849" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C849" t="s">
-        <v>335</v>
+        <v>421</v>
       </c>
       <c r="D849">
         <v>780</v>
       </c>
       <c r="E849" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="F849" t="s">
         <v>102</v>
@@ -28830,19 +28833,19 @@
     </row>
     <row r="850" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A850" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
       <c r="B850" s="2" t="s">
-        <v>690</v>
+        <v>117</v>
       </c>
       <c r="C850" t="s">
         <v>335</v>
       </c>
       <c r="D850">
-        <v>960</v>
+        <v>780</v>
       </c>
       <c r="E850" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="F850" t="s">
         <v>102</v>
@@ -28856,236 +28859,236 @@
     </row>
     <row r="851" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A851" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="B851" s="2" t="s">
-        <v>803</v>
+        <v>690</v>
       </c>
       <c r="C851" t="s">
-        <v>1932</v>
+        <v>335</v>
       </c>
       <c r="D851">
-        <v>137</v>
+        <v>960</v>
       </c>
       <c r="E851" t="s">
-        <v>758</v>
+        <v>1930</v>
       </c>
       <c r="F851" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="G851" t="s">
-        <v>58</v>
+        <v>1844</v>
       </c>
       <c r="H851" s="1">
-        <v>43232</v>
+        <v>43431</v>
       </c>
     </row>
     <row r="852" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A852" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="B852" s="2" t="s">
-        <v>155</v>
+        <v>803</v>
       </c>
       <c r="C852" t="s">
-        <v>596</v>
+        <v>1932</v>
       </c>
       <c r="D852">
-        <v>82</v>
+        <v>137</v>
       </c>
       <c r="E852" t="s">
-        <v>1289</v>
+        <v>758</v>
       </c>
       <c r="F852" t="s">
         <v>12</v>
       </c>
       <c r="G852" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="H852" s="1">
-        <v>43268</v>
+        <v>43232</v>
       </c>
     </row>
     <row r="853" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A853" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B853" s="2" t="s">
-        <v>275</v>
+        <v>155</v>
       </c>
       <c r="C853" t="s">
-        <v>1935</v>
+        <v>596</v>
       </c>
       <c r="D853">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E853" t="s">
-        <v>1936</v>
+        <v>1289</v>
       </c>
       <c r="F853" t="s">
         <v>12</v>
       </c>
       <c r="G853" t="s">
-        <v>194</v>
+        <v>13</v>
       </c>
       <c r="H853" s="1">
-        <v>43197</v>
+        <v>43268</v>
       </c>
     </row>
     <row r="854" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A854" t="s">
-        <v>1937</v>
+        <v>1934</v>
       </c>
       <c r="B854" s="2" t="s">
-        <v>1938</v>
+        <v>275</v>
       </c>
       <c r="C854" t="s">
-        <v>1939</v>
+        <v>1935</v>
       </c>
       <c r="D854">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="E854" t="s">
-        <v>1940</v>
+        <v>1936</v>
       </c>
       <c r="F854" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G854" t="s">
-        <v>507</v>
+        <v>194</v>
       </c>
       <c r="H854" s="1">
-        <v>43453</v>
+        <v>43197</v>
       </c>
     </row>
     <row r="855" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A855" t="s">
-        <v>1941</v>
+        <v>1937</v>
       </c>
       <c r="B855" s="2" t="s">
-        <v>29</v>
+        <v>1938</v>
       </c>
       <c r="C855" t="s">
-        <v>146</v>
+        <v>1939</v>
       </c>
       <c r="D855">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="E855" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="F855" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G855" t="s">
-        <v>1710</v>
+        <v>507</v>
       </c>
       <c r="H855" s="1">
-        <v>43115</v>
+        <v>43453</v>
       </c>
     </row>
     <row r="856" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A856" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="B856" s="2" t="s">
-        <v>645</v>
+        <v>29</v>
       </c>
       <c r="C856" t="s">
-        <v>1944</v>
+        <v>146</v>
       </c>
       <c r="D856">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E856" t="s">
-        <v>50</v>
+        <v>1942</v>
       </c>
       <c r="F856" t="s">
         <v>12</v>
       </c>
       <c r="G856" t="s">
-        <v>13</v>
+        <v>1710</v>
       </c>
       <c r="H856" s="1">
-        <v>43424</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="857" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A857" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="B857" s="2" t="s">
-        <v>1946</v>
+        <v>645</v>
       </c>
       <c r="C857" t="s">
-        <v>1947</v>
+        <v>1944</v>
       </c>
       <c r="D857">
-        <v>130</v>
+        <v>89</v>
       </c>
       <c r="E857" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F857" t="s">
         <v>12</v>
       </c>
       <c r="G857" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="H857" s="1">
-        <v>43180</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="858" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A858" t="s">
-        <v>1948</v>
+        <v>1945</v>
       </c>
       <c r="B858" s="2" t="s">
-        <v>275</v>
+        <v>1946</v>
       </c>
       <c r="C858" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="D858">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="E858" t="s">
-        <v>1950</v>
+        <v>57</v>
       </c>
       <c r="F858" t="s">
         <v>12</v>
       </c>
       <c r="G858" t="s">
-        <v>1951</v>
+        <v>79</v>
       </c>
       <c r="H858" s="1">
-        <v>43115</v>
+        <v>43180</v>
       </c>
     </row>
     <row r="859" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A859" t="s">
-        <v>1952</v>
+        <v>1948</v>
       </c>
       <c r="B859" s="2" t="s">
         <v>275</v>
       </c>
       <c r="C859" t="s">
-        <v>1953</v>
+        <v>1949</v>
       </c>
       <c r="D859">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E859" t="s">
         <v>1950</v>
       </c>
       <c r="F859" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G859" t="s">
-        <v>13</v>
+        <v>1951</v>
       </c>
       <c r="H859" s="1">
-        <v>43894</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="860" spans="1:8" x14ac:dyDescent="0.3">
@@ -29108,163 +29111,163 @@
         <v>37</v>
       </c>
       <c r="G860" t="s">
-        <v>1651</v>
+        <v>13</v>
       </c>
       <c r="H860" s="1">
-        <v>44891</v>
+        <v>43894</v>
       </c>
     </row>
     <row r="861" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A861" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="B861" s="2" t="s">
         <v>275</v>
       </c>
       <c r="C861" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="D861">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E861" t="s">
-        <v>78</v>
+        <v>1950</v>
       </c>
       <c r="F861" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G861" t="s">
-        <v>431</v>
+        <v>1651</v>
       </c>
       <c r="H861" s="1">
-        <v>43115</v>
+        <v>44891</v>
       </c>
     </row>
     <row r="862" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A862" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="B862" s="2" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="C862" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="D862">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="E862" t="s">
-        <v>515</v>
+        <v>78</v>
       </c>
       <c r="F862" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G862" t="s">
-        <v>1392</v>
+        <v>431</v>
       </c>
       <c r="H862" s="1">
-        <v>43139</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="863" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A863" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="B863" s="2" t="s">
-        <v>476</v>
+        <v>136</v>
       </c>
       <c r="C863" t="s">
-        <v>775</v>
+        <v>1957</v>
       </c>
       <c r="D863">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="E863" t="s">
-        <v>1882</v>
+        <v>515</v>
       </c>
       <c r="F863" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G863" t="s">
-        <v>164</v>
+        <v>1392</v>
       </c>
       <c r="H863" s="1">
-        <v>43834</v>
+        <v>43139</v>
       </c>
     </row>
     <row r="864" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A864" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B864" s="2" t="s">
-        <v>9</v>
+        <v>476</v>
       </c>
       <c r="C864" t="s">
-        <v>1960</v>
+        <v>775</v>
       </c>
       <c r="D864">
-        <v>162</v>
+        <v>101</v>
       </c>
       <c r="E864" t="s">
-        <v>1961</v>
+        <v>1882</v>
       </c>
       <c r="F864" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G864" t="s">
-        <v>13</v>
+        <v>164</v>
       </c>
       <c r="H864" s="1">
-        <v>43134</v>
+        <v>43834</v>
       </c>
     </row>
     <row r="865" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A865" t="s">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="B865" s="2" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
       <c r="C865" t="s">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="D865">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="E865" t="s">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="F865" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G865" t="s">
-        <v>198</v>
+        <v>13</v>
       </c>
       <c r="H865" s="1">
-        <v>43115</v>
+        <v>43134</v>
       </c>
     </row>
     <row r="866" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A866" t="s">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="B866" s="2" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="C866" t="s">
-        <v>1966</v>
+        <v>1963</v>
       </c>
       <c r="D866">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E866" t="s">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="F866" t="s">
         <v>12</v>
       </c>
       <c r="G866" t="s">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="H866" s="1">
         <v>43115</v>
@@ -29272,149 +29275,149 @@
     </row>
     <row r="867" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A867" t="s">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="B867" s="2" t="s">
-        <v>1969</v>
+        <v>109</v>
       </c>
       <c r="C867" t="s">
-        <v>438</v>
+        <v>1966</v>
       </c>
       <c r="D867">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="E867" t="s">
-        <v>1737</v>
+        <v>1967</v>
       </c>
       <c r="F867" t="s">
         <v>12</v>
       </c>
       <c r="G867" t="s">
-        <v>1511</v>
+        <v>13</v>
       </c>
       <c r="H867" s="1">
-        <v>43154</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="868" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A868" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="B868" s="2" t="s">
-        <v>15</v>
+        <v>1969</v>
       </c>
       <c r="C868" t="s">
-        <v>1971</v>
+        <v>438</v>
       </c>
       <c r="D868">
-        <v>600</v>
+        <v>110</v>
       </c>
       <c r="E868" t="s">
-        <v>1972</v>
+        <v>1737</v>
       </c>
       <c r="F868" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G868" t="s">
-        <v>13</v>
+        <v>1511</v>
       </c>
       <c r="H868" s="1">
-        <v>43227</v>
+        <v>43154</v>
       </c>
     </row>
     <row r="869" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A869" t="s">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="B869" s="2" t="s">
-        <v>1974</v>
+        <v>15</v>
       </c>
       <c r="C869" t="s">
-        <v>596</v>
+        <v>1971</v>
       </c>
       <c r="D869">
-        <v>86</v>
+        <v>600</v>
       </c>
       <c r="E869" t="s">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="F869" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G869" t="s">
         <v>13</v>
       </c>
       <c r="H869" s="1">
-        <v>43303</v>
+        <v>43227</v>
       </c>
     </row>
     <row r="870" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A870" t="s">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B870" s="2" t="s">
-        <v>792</v>
+        <v>1974</v>
       </c>
       <c r="C870" t="s">
-        <v>146</v>
+        <v>596</v>
       </c>
       <c r="D870">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="E870" t="s">
-        <v>1977</v>
+        <v>1975</v>
       </c>
       <c r="F870" t="s">
         <v>12</v>
       </c>
       <c r="G870" t="s">
-        <v>107</v>
+        <v>13</v>
       </c>
       <c r="H870" s="1">
-        <v>43434</v>
+        <v>43303</v>
       </c>
     </row>
     <row r="871" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="B871" s="2" t="s">
-        <v>43</v>
+        <v>792</v>
       </c>
       <c r="C871" t="s">
-        <v>1550</v>
+        <v>146</v>
       </c>
       <c r="D871">
-        <v>158</v>
+        <v>104</v>
       </c>
       <c r="E871" t="s">
-        <v>1147</v>
+        <v>1977</v>
       </c>
       <c r="F871" t="s">
         <v>12</v>
       </c>
       <c r="G871" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="H871" s="1">
-        <v>43271</v>
+        <v>43434</v>
       </c>
     </row>
     <row r="872" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B872" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C872" t="s">
-        <v>1980</v>
+        <v>1550</v>
       </c>
       <c r="D872">
-        <v>131</v>
+        <v>158</v>
       </c>
       <c r="E872" t="s">
-        <v>1077</v>
+        <v>1147</v>
       </c>
       <c r="F872" t="s">
         <v>12</v>
@@ -29428,94 +29431,94 @@
     </row>
     <row r="873" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
-        <v>1981</v>
+        <v>1979</v>
       </c>
       <c r="B873" s="2" t="s">
-        <v>826</v>
+        <v>63</v>
       </c>
       <c r="C873" t="s">
-        <v>1982</v>
+        <v>1980</v>
       </c>
       <c r="D873">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="E873" t="s">
-        <v>541</v>
+        <v>1077</v>
       </c>
       <c r="F873" t="s">
         <v>12</v>
       </c>
       <c r="G873" t="s">
-        <v>1983</v>
+        <v>13</v>
       </c>
       <c r="H873" s="1">
-        <v>43229</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="874" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="B874" s="2" t="s">
-        <v>448</v>
+        <v>826</v>
       </c>
       <c r="C874" t="s">
-        <v>1150</v>
+        <v>1982</v>
       </c>
       <c r="D874">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="E874" t="s">
-        <v>273</v>
+        <v>541</v>
       </c>
       <c r="F874" t="s">
         <v>12</v>
       </c>
       <c r="G874" t="s">
-        <v>46</v>
+        <v>1983</v>
       </c>
       <c r="H874" s="1">
-        <v>43224</v>
+        <v>43229</v>
       </c>
     </row>
     <row r="875" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B875" s="2" t="s">
-        <v>1451</v>
+        <v>448</v>
       </c>
       <c r="C875" t="s">
-        <v>49</v>
+        <v>1150</v>
       </c>
       <c r="D875">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="E875" t="s">
-        <v>50</v>
+        <v>273</v>
       </c>
       <c r="F875" t="s">
         <v>12</v>
       </c>
       <c r="G875" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="H875" s="1">
-        <v>43424</v>
+        <v>43224</v>
       </c>
     </row>
     <row r="876" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B876" s="2" t="s">
-        <v>1021</v>
+        <v>1451</v>
       </c>
       <c r="C876" t="s">
         <v>49</v>
       </c>
       <c r="D876">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="E876" t="s">
         <v>50</v>
@@ -29532,19 +29535,19 @@
     </row>
     <row r="877" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B877" s="2" t="s">
-        <v>63</v>
+        <v>1021</v>
       </c>
       <c r="C877" t="s">
-        <v>1988</v>
+        <v>49</v>
       </c>
       <c r="D877">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="E877" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F877" t="s">
         <v>12</v>
@@ -29553,59 +29556,59 @@
         <v>13</v>
       </c>
       <c r="H877" s="1">
-        <v>43186</v>
+        <v>43424</v>
       </c>
     </row>
     <row r="878" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
       <c r="B878" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C878" t="s">
-        <v>137</v>
+        <v>1988</v>
       </c>
       <c r="D878">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E878" t="s">
-        <v>1533</v>
+        <v>57</v>
       </c>
       <c r="F878" t="s">
         <v>12</v>
       </c>
       <c r="G878" t="s">
-        <v>756</v>
+        <v>13</v>
       </c>
       <c r="H878" s="1">
-        <v>43121</v>
+        <v>43186</v>
       </c>
     </row>
     <row r="879" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B879" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C879" t="s">
-        <v>1294</v>
+        <v>137</v>
       </c>
       <c r="D879">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="E879" t="s">
-        <v>255</v>
+        <v>1533</v>
       </c>
       <c r="F879" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G879" t="s">
-        <v>13</v>
+        <v>756</v>
       </c>
       <c r="H879" s="1">
-        <v>43816</v>
+        <v>43121</v>
       </c>
     </row>
     <row r="880" spans="1:8" x14ac:dyDescent="0.3">
@@ -29625,65 +29628,65 @@
         <v>255</v>
       </c>
       <c r="F880" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G880" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H880" s="1">
-        <v>43115</v>
+        <v>43816</v>
       </c>
     </row>
     <row r="881" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A881" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B881" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C881" t="s">
-        <v>1992</v>
+        <v>1294</v>
       </c>
       <c r="D881">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E881" t="s">
-        <v>1993</v>
+        <v>255</v>
       </c>
       <c r="F881" t="s">
         <v>12</v>
       </c>
       <c r="G881" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H881" s="1">
-        <v>43523</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="882" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A882" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="B882" s="2" t="s">
-        <v>1995</v>
+        <v>76</v>
       </c>
       <c r="C882" t="s">
-        <v>517</v>
+        <v>1992</v>
       </c>
       <c r="D882">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E882" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="F882" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G882" t="s">
-        <v>204</v>
+        <v>13</v>
       </c>
       <c r="H882" s="1">
-        <v>43874</v>
+        <v>43523</v>
       </c>
     </row>
     <row r="883" spans="1:8" x14ac:dyDescent="0.3">
@@ -29694,7 +29697,7 @@
         <v>1995</v>
       </c>
       <c r="C883" t="s">
-        <v>809</v>
+        <v>517</v>
       </c>
       <c r="D883">
         <v>101</v>
@@ -29703,56 +29706,56 @@
         <v>1996</v>
       </c>
       <c r="F883" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="G883" t="s">
         <v>204</v>
       </c>
       <c r="H883" s="1">
-        <v>43115</v>
+        <v>43874</v>
       </c>
     </row>
     <row r="884" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A884" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="B884" s="2" t="s">
-        <v>502</v>
+        <v>1995</v>
       </c>
       <c r="C884" t="s">
-        <v>1998</v>
+        <v>809</v>
       </c>
       <c r="D884">
-        <v>191</v>
+        <v>101</v>
       </c>
       <c r="E884" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="F884" t="s">
         <v>12</v>
       </c>
       <c r="G884" t="s">
-        <v>13</v>
+        <v>204</v>
       </c>
       <c r="H884" s="1">
-        <v>43271</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="885" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A885" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="B885" s="2" t="s">
-        <v>795</v>
+        <v>502</v>
       </c>
       <c r="C885" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="D885">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="E885" t="s">
-        <v>387</v>
+        <v>1999</v>
       </c>
       <c r="F885" t="s">
         <v>12</v>
@@ -29761,21 +29764,21 @@
         <v>13</v>
       </c>
       <c r="H885" s="1">
-        <v>43186</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="886" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A886" t="s">
-        <v>2002</v>
+        <v>2000</v>
       </c>
       <c r="B886" s="2" t="s">
-        <v>177</v>
+        <v>795</v>
       </c>
       <c r="C886" t="s">
-        <v>246</v>
+        <v>2001</v>
       </c>
       <c r="D886">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="E886" t="s">
         <v>387</v>
@@ -29792,71 +29795,71 @@
     </row>
     <row r="887" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A887" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B887" s="2" t="s">
-        <v>29</v>
+        <v>177</v>
       </c>
       <c r="C887" t="s">
         <v>246</v>
       </c>
       <c r="D887">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E887" t="s">
-        <v>1153</v>
+        <v>387</v>
       </c>
       <c r="F887" t="s">
         <v>12</v>
       </c>
       <c r="G887" t="s">
-        <v>153</v>
+        <v>13</v>
       </c>
       <c r="H887" s="1">
-        <v>43115</v>
+        <v>43186</v>
       </c>
     </row>
     <row r="888" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A888" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B888" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C888" t="s">
-        <v>2005</v>
+        <v>246</v>
       </c>
       <c r="D888">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="E888" t="s">
-        <v>2006</v>
+        <v>1153</v>
       </c>
       <c r="F888" t="s">
         <v>12</v>
       </c>
       <c r="G888" t="s">
-        <v>13</v>
+        <v>153</v>
       </c>
       <c r="H888" s="1">
-        <v>43186</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="889" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A889" t="s">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="B889" s="2" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="C889" t="s">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="D889">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="E889" t="s">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="F889" t="s">
         <v>12</v>
@@ -29870,80 +29873,80 @@
     </row>
     <row r="890" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A890" t="s">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="B890" s="2" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="C890" t="s">
-        <v>928</v>
+        <v>2008</v>
       </c>
       <c r="D890">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="E890" t="s">
-        <v>906</v>
+        <v>2009</v>
       </c>
       <c r="F890" t="s">
         <v>12</v>
       </c>
       <c r="G890" t="s">
-        <v>168</v>
+        <v>13</v>
       </c>
       <c r="H890" s="1">
-        <v>43197</v>
+        <v>43186</v>
       </c>
     </row>
     <row r="891" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A891" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B891" s="2" t="s">
-        <v>275</v>
+        <v>9</v>
       </c>
       <c r="C891" t="s">
-        <v>146</v>
+        <v>928</v>
       </c>
       <c r="D891">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E891" t="s">
-        <v>203</v>
+        <v>906</v>
       </c>
       <c r="F891" t="s">
         <v>12</v>
       </c>
       <c r="G891" t="s">
-        <v>46</v>
+        <v>168</v>
       </c>
       <c r="H891" s="1">
-        <v>43225</v>
+        <v>43197</v>
       </c>
     </row>
     <row r="892" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A892" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B892" s="2" t="s">
-        <v>48</v>
+        <v>275</v>
       </c>
       <c r="C892" t="s">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="D892">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E892" t="s">
-        <v>1650</v>
+        <v>203</v>
       </c>
       <c r="F892" t="s">
         <v>12</v>
       </c>
       <c r="G892" t="s">
-        <v>1651</v>
+        <v>46</v>
       </c>
       <c r="H892" s="1">
-        <v>44925</v>
+        <v>43225</v>
       </c>
     </row>
     <row r="893" spans="1:8" x14ac:dyDescent="0.3">
@@ -29974,103 +29977,103 @@
     </row>
     <row r="894" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A894" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B894" s="2" t="s">
-        <v>275</v>
+        <v>48</v>
       </c>
       <c r="C894" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="D894">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E894" t="s">
-        <v>2014</v>
+        <v>1650</v>
       </c>
       <c r="F894" t="s">
         <v>12</v>
       </c>
       <c r="G894" t="s">
-        <v>194</v>
+        <v>1651</v>
       </c>
       <c r="H894" s="1">
-        <v>43197</v>
+        <v>44925</v>
       </c>
     </row>
     <row r="895" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A895" t="s">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="B895" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C895" t="s">
+        <v>207</v>
+      </c>
+      <c r="D895">
         <v>117</v>
       </c>
-      <c r="C895" t="s">
-        <v>596</v>
-      </c>
-      <c r="D895">
-        <v>106</v>
-      </c>
       <c r="E895" t="s">
-        <v>373</v>
+        <v>2014</v>
       </c>
       <c r="F895" t="s">
         <v>12</v>
       </c>
       <c r="G895" t="s">
-        <v>13</v>
+        <v>194</v>
       </c>
       <c r="H895" s="1">
-        <v>43271</v>
+        <v>43197</v>
       </c>
     </row>
     <row r="896" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A896" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B896" s="2" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="C896" t="s">
-        <v>1135</v>
+        <v>596</v>
       </c>
       <c r="D896">
         <v>106</v>
       </c>
       <c r="E896" t="s">
-        <v>2017</v>
+        <v>373</v>
       </c>
       <c r="F896" t="s">
         <v>12</v>
       </c>
       <c r="G896" t="s">
-        <v>164</v>
+        <v>13</v>
       </c>
       <c r="H896" s="1">
-        <v>43306</v>
+        <v>43271</v>
       </c>
     </row>
     <row r="897" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A897" t="s">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B897" s="2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="C897" t="s">
-        <v>171</v>
+        <v>1135</v>
       </c>
       <c r="D897">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="E897" t="s">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="F897" t="s">
         <v>12</v>
       </c>
       <c r="G897" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="H897" s="1">
         <v>43306</v>
@@ -30078,59 +30081,59 @@
     </row>
     <row r="898" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A898" t="s">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="B898" s="2" t="s">
-        <v>275</v>
+        <v>9</v>
       </c>
       <c r="C898" t="s">
         <v>171</v>
       </c>
       <c r="D898">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="E898" t="s">
-        <v>649</v>
+        <v>2019</v>
       </c>
       <c r="F898" t="s">
         <v>12</v>
       </c>
       <c r="G898" t="s">
-        <v>948</v>
+        <v>168</v>
       </c>
       <c r="H898" s="1">
-        <v>43225</v>
+        <v>43306</v>
       </c>
     </row>
     <row r="899" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A899" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B899" s="2" t="s">
-        <v>1021</v>
+        <v>275</v>
       </c>
       <c r="C899" t="s">
-        <v>2022</v>
+        <v>171</v>
       </c>
       <c r="D899">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="E899" t="s">
-        <v>2023</v>
+        <v>649</v>
       </c>
       <c r="F899" t="s">
         <v>12</v>
       </c>
       <c r="G899" t="s">
-        <v>13</v>
+        <v>948</v>
       </c>
       <c r="H899" s="1">
-        <v>43564</v>
+        <v>43225</v>
       </c>
     </row>
     <row r="900" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A900" t="s">
-        <v>2024</v>
+        <v>2021</v>
       </c>
       <c r="B900" s="2" t="s">
         <v>1021</v>
@@ -30139,10 +30142,10 @@
         <v>2022</v>
       </c>
       <c r="D900">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="E900" t="s">
-        <v>2025</v>
+        <v>2023</v>
       </c>
       <c r="F900" t="s">
         <v>12</v>
@@ -30156,19 +30159,19 @@
     </row>
     <row r="901" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A901" t="s">
-        <v>2026</v>
+        <v>2024</v>
       </c>
       <c r="B901" s="2" t="s">
-        <v>881</v>
+        <v>1021</v>
       </c>
       <c r="C901" t="s">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="D901">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E901" t="s">
-        <v>2028</v>
+        <v>2025</v>
       </c>
       <c r="F901" t="s">
         <v>12</v>
@@ -30182,7 +30185,7 @@
     </row>
     <row r="902" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A902" t="s">
-        <v>2029</v>
+        <v>2026</v>
       </c>
       <c r="B902" s="2" t="s">
         <v>881</v>
@@ -30191,7 +30194,7 @@
         <v>2027</v>
       </c>
       <c r="D902">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E902" t="s">
         <v>2028</v>
@@ -30208,19 +30211,19 @@
     </row>
     <row r="903" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A903" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B903" s="2" t="s">
         <v>881</v>
       </c>
       <c r="C903" t="s">
-        <v>2031</v>
+        <v>2027</v>
       </c>
       <c r="D903">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E903" t="s">
-        <v>2032</v>
+        <v>2028</v>
       </c>
       <c r="F903" t="s">
         <v>12</v>
@@ -30234,19 +30237,19 @@
     </row>
     <row r="904" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A904" t="s">
-        <v>2033</v>
+        <v>2030</v>
       </c>
       <c r="B904" s="2" t="s">
-        <v>145</v>
+        <v>881</v>
       </c>
       <c r="C904" t="s">
-        <v>2027</v>
+        <v>2031</v>
       </c>
       <c r="D904">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E904" t="s">
-        <v>2034</v>
+        <v>2032</v>
       </c>
       <c r="F904" t="s">
         <v>12</v>
@@ -30260,7 +30263,7 @@
     </row>
     <row r="905" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A905" t="s">
-        <v>2035</v>
+        <v>2033</v>
       </c>
       <c r="B905" s="2" t="s">
         <v>145</v>
@@ -30286,7 +30289,7 @@
     </row>
     <row r="906" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A906" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B906" s="2" t="s">
         <v>145</v>
@@ -30298,7 +30301,7 @@
         <v>82</v>
       </c>
       <c r="E906" t="s">
-        <v>2023</v>
+        <v>2034</v>
       </c>
       <c r="F906" t="s">
         <v>12</v>
@@ -30312,19 +30315,19 @@
     </row>
     <row r="907" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A907" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B907" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C907" t="s">
-        <v>2038</v>
+        <v>2027</v>
       </c>
       <c r="D907">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E907" t="s">
-        <v>2032</v>
+        <v>2023</v>
       </c>
       <c r="F907" t="s">
         <v>12</v>
@@ -30338,19 +30341,19 @@
     </row>
     <row r="908" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A908" t="s">
-        <v>2039</v>
+        <v>2037</v>
       </c>
       <c r="B908" s="2" t="s">
-        <v>792</v>
+        <v>145</v>
       </c>
       <c r="C908" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="D908">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E908" t="s">
-        <v>2041</v>
+        <v>2032</v>
       </c>
       <c r="F908" t="s">
         <v>12</v>
@@ -30364,19 +30367,19 @@
     </row>
     <row r="909" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A909" t="s">
-        <v>2042</v>
+        <v>2039</v>
       </c>
       <c r="B909" s="2" t="s">
         <v>792</v>
       </c>
       <c r="C909" t="s">
-        <v>2027</v>
+        <v>2040</v>
       </c>
       <c r="D909">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="E909" t="s">
-        <v>2025</v>
+        <v>2041</v>
       </c>
       <c r="F909" t="s">
         <v>12</v>
@@ -30390,7 +30393,7 @@
     </row>
     <row r="910" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A910" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B910" s="2" t="s">
         <v>792</v>
@@ -30399,10 +30402,10 @@
         <v>2027</v>
       </c>
       <c r="D910">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E910" t="s">
-        <v>2023</v>
+        <v>2025</v>
       </c>
       <c r="F910" t="s">
         <v>12</v>
@@ -30416,19 +30419,19 @@
     </row>
     <row r="911" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A911" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B911" s="2" t="s">
-        <v>104</v>
+        <v>792</v>
       </c>
       <c r="C911" t="s">
         <v>2027</v>
       </c>
       <c r="D911">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="E911" t="s">
-        <v>2028</v>
+        <v>2023</v>
       </c>
       <c r="F911" t="s">
         <v>12</v>
@@ -30442,19 +30445,19 @@
     </row>
     <row r="912" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A912" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B912" s="2" t="s">
         <v>104</v>
       </c>
       <c r="C912" t="s">
-        <v>551</v>
+        <v>2027</v>
       </c>
       <c r="D912">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E912" t="s">
-        <v>2034</v>
+        <v>2028</v>
       </c>
       <c r="F912" t="s">
         <v>12</v>
@@ -30468,19 +30471,19 @@
     </row>
     <row r="913" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A913" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B913" s="2" t="s">
-        <v>305</v>
+        <v>104</v>
       </c>
       <c r="C913" t="s">
-        <v>2027</v>
+        <v>551</v>
       </c>
       <c r="D913">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E913" t="s">
-        <v>2032</v>
+        <v>2034</v>
       </c>
       <c r="F913" t="s">
         <v>12</v>
@@ -30494,19 +30497,19 @@
     </row>
     <row r="914" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A914" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B914" s="2" t="s">
-        <v>476</v>
+        <v>305</v>
       </c>
       <c r="C914" t="s">
-        <v>1253</v>
+        <v>2027</v>
       </c>
       <c r="D914">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E914" t="s">
-        <v>2048</v>
+        <v>2032</v>
       </c>
       <c r="F914" t="s">
         <v>12</v>
@@ -30520,19 +30523,19 @@
     </row>
     <row r="915" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A915" t="s">
-        <v>2049</v>
+        <v>2047</v>
       </c>
       <c r="B915" s="2" t="s">
         <v>476</v>
       </c>
       <c r="C915" t="s">
-        <v>2040</v>
+        <v>1253</v>
       </c>
       <c r="D915">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="E915" t="s">
-        <v>2023</v>
+        <v>2048</v>
       </c>
       <c r="F915" t="s">
         <v>12</v>
@@ -30546,19 +30549,19 @@
     </row>
     <row r="916" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A916" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B916" s="2" t="s">
-        <v>43</v>
+        <v>476</v>
       </c>
       <c r="C916" t="s">
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="D916">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E916" t="s">
-        <v>2032</v>
+        <v>2023</v>
       </c>
       <c r="F916" t="s">
         <v>12</v>
@@ -30572,19 +30575,19 @@
     </row>
     <row r="917" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A917" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B917" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C917" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="D917">
         <v>82</v>
       </c>
       <c r="E917" t="s">
-        <v>2023</v>
+        <v>2032</v>
       </c>
       <c r="F917" t="s">
         <v>12</v>
@@ -30598,19 +30601,19 @@
     </row>
     <row r="918" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A918" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B918" s="2" t="s">
-        <v>113</v>
+        <v>43</v>
       </c>
       <c r="C918" t="s">
-        <v>2038</v>
+        <v>2040</v>
       </c>
       <c r="D918">
-        <v>115</v>
+        <v>82</v>
       </c>
       <c r="E918" t="s">
-        <v>2053</v>
+        <v>2023</v>
       </c>
       <c r="F918" t="s">
         <v>12</v>
@@ -30624,19 +30627,19 @@
     </row>
     <row r="919" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A919" t="s">
-        <v>2054</v>
+        <v>2052</v>
       </c>
       <c r="B919" s="2" t="s">
         <v>113</v>
       </c>
       <c r="C919" t="s">
-        <v>2040</v>
+        <v>2038</v>
       </c>
       <c r="D919">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="E919" t="s">
-        <v>2023</v>
+        <v>2053</v>
       </c>
       <c r="F919" t="s">
         <v>12</v>
@@ -30650,19 +30653,19 @@
     </row>
     <row r="920" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A920" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B920" s="2" t="s">
-        <v>305</v>
+        <v>113</v>
       </c>
       <c r="C920" t="s">
-        <v>2027</v>
+        <v>2040</v>
       </c>
       <c r="D920">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E920" t="s">
-        <v>2032</v>
+        <v>2023</v>
       </c>
       <c r="F920" t="s">
         <v>12</v>
@@ -30676,19 +30679,19 @@
     </row>
     <row r="921" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A921" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="B921" s="2" t="s">
-        <v>538</v>
+        <v>305</v>
       </c>
       <c r="C921" t="s">
-        <v>2040</v>
+        <v>2027</v>
       </c>
       <c r="D921">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E921" t="s">
-        <v>2025</v>
+        <v>2032</v>
       </c>
       <c r="F921" t="s">
         <v>12</v>
@@ -30702,19 +30705,19 @@
     </row>
     <row r="922" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A922" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B922" s="2" t="s">
         <v>538</v>
       </c>
       <c r="C922" t="s">
-        <v>2058</v>
+        <v>2040</v>
       </c>
       <c r="D922">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E922" t="s">
-        <v>2059</v>
+        <v>2025</v>
       </c>
       <c r="F922" t="s">
         <v>12</v>
@@ -30728,19 +30731,19 @@
     </row>
     <row r="923" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A923" t="s">
-        <v>2060</v>
+        <v>2057</v>
       </c>
       <c r="B923" s="2" t="s">
-        <v>161</v>
+        <v>538</v>
       </c>
       <c r="C923" t="s">
-        <v>2061</v>
+        <v>2058</v>
       </c>
       <c r="D923">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E923" t="s">
-        <v>2032</v>
+        <v>2059</v>
       </c>
       <c r="F923" t="s">
         <v>12</v>
@@ -30754,79 +30757,105 @@
     </row>
     <row r="924" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A924" t="s">
-        <v>2062</v>
+        <v>2060</v>
       </c>
       <c r="B924" s="2" t="s">
-        <v>9</v>
+        <v>161</v>
       </c>
       <c r="C924" t="s">
-        <v>1273</v>
+        <v>2061</v>
       </c>
       <c r="D924">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E924" t="s">
-        <v>1940</v>
+        <v>2032</v>
       </c>
       <c r="F924" t="s">
         <v>12</v>
       </c>
       <c r="G924" t="s">
-        <v>507</v>
+        <v>13</v>
       </c>
       <c r="H924" s="1">
-        <v>43115</v>
+        <v>43564</v>
       </c>
     </row>
     <row r="925" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A925" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B925" s="2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C925" t="s">
         <v>1273</v>
       </c>
       <c r="D925">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E925" t="s">
         <v>1940</v>
       </c>
       <c r="F925" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="G925" t="s">
-        <v>13</v>
+        <v>507</v>
       </c>
       <c r="H925" s="1">
-        <v>43854</v>
+        <v>43115</v>
       </c>
     </row>
     <row r="926" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A926" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B926" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C926" t="s">
+        <v>1273</v>
+      </c>
+      <c r="D926">
+        <v>99</v>
+      </c>
+      <c r="E926" t="s">
+        <v>1940</v>
+      </c>
+      <c r="F926" t="s">
+        <v>37</v>
+      </c>
+      <c r="G926" t="s">
+        <v>13</v>
+      </c>
+      <c r="H926" s="1">
+        <v>43854</v>
+      </c>
+    </row>
+    <row r="927" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A927" t="s">
         <v>2064</v>
       </c>
-      <c r="B926" s="2" t="s">
+      <c r="B927" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C926" t="s">
+      <c r="C927" t="s">
         <v>424</v>
       </c>
-      <c r="D926">
+      <c r="D927">
         <v>139</v>
       </c>
-      <c r="E926" t="s">
+      <c r="E927" t="s">
         <v>2065</v>
       </c>
-      <c r="F926" t="s">
-        <v>12</v>
-      </c>
-      <c r="G926" t="s">
+      <c r="F927" t="s">
+        <v>12</v>
+      </c>
+      <c r="G927" t="s">
         <v>756</v>
       </c>
-      <c r="H926" s="1">
+      <c r="H927" s="1">
         <v>43195</v>
       </c>
     </row>

</xml_diff>